<commit_message>
making it so running the savings project does not save the excel sheet to github
</commit_message>
<xml_diff>
--- a/Python/saving tracking/expenses.xlsx
+++ b/Python/saving tracking/expenses.xlsx
@@ -468,7 +468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -578,6 +578,26 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-02-05</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>clothes</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>250</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Work</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>